<commit_message>
update to consultancy mode
</commit_message>
<xml_diff>
--- a/name_generator/dict/algorithms/algorithm_list.xlsx
+++ b/name_generator/dict/algorithms/algorithm_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/masayukikishi/Dropbox (Personal)/masayuki_kishi/repositories/create_names_v2/name_generator/dict/algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5219C98-CF69-1B4D-992E-C6AB1B2A0DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A0476A-204B-174D-9D44-32F53524F99F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="algorithms" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">algorithms!$B$1:$H$509</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">algorithms!$B$1:$G$118</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">backup!$B$1:$G$259</definedName>
     <definedName name="algorithms_combined_2x2">[1]algorithms_combined!$B$2:$AA$22</definedName>
     <definedName name="algorithms_combined_3x3">[1]algorithms_combined!$AE$2:$CJ$91</definedName>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3235" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3293" uniqueCount="38">
   <si>
     <t>keyword_type_1</t>
   </si>
@@ -18721,8 +18721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AML118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M122" sqref="M122"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -19846,7 +19846,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>47</v>
       </c>
@@ -19869,7 +19869,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>48</v>
       </c>
@@ -19892,7 +19892,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>49</v>
       </c>
@@ -19914,8 +19914,11 @@
       <c r="G51" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H51" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>50</v>
       </c>
@@ -19937,8 +19940,11 @@
       <c r="G52" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H52" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>51</v>
       </c>
@@ -19960,8 +19966,11 @@
       <c r="G53" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H53" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>52</v>
       </c>
@@ -19983,8 +19992,11 @@
       <c r="G54" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H54" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>53</v>
       </c>
@@ -20006,8 +20018,11 @@
       <c r="G55" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H55" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>54</v>
       </c>
@@ -20029,8 +20044,11 @@
       <c r="G56" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H56" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>55</v>
       </c>
@@ -20052,8 +20070,11 @@
       <c r="G57" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H57" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>56</v>
       </c>
@@ -20075,8 +20096,11 @@
       <c r="G58" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H58" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>57</v>
       </c>
@@ -20098,8 +20122,11 @@
       <c r="G59" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H59" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>58</v>
       </c>
@@ -20121,8 +20148,11 @@
       <c r="G60" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H60" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>59</v>
       </c>
@@ -20144,8 +20174,11 @@
       <c r="G61" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H61" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>60</v>
       </c>
@@ -20167,8 +20200,11 @@
       <c r="G62" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H62" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>61</v>
       </c>
@@ -20190,8 +20226,11 @@
       <c r="G63" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H63" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>62</v>
       </c>
@@ -20214,7 +20253,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>63</v>
       </c>
@@ -20237,7 +20276,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>64</v>
       </c>
@@ -20259,8 +20298,11 @@
       <c r="G66" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H66" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>65</v>
       </c>
@@ -20283,7 +20325,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>66</v>
       </c>
@@ -20305,8 +20347,11 @@
       <c r="G68" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H68" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>67</v>
       </c>
@@ -20329,7 +20374,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>68</v>
       </c>
@@ -20351,8 +20396,11 @@
       <c r="G70" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H70" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>69</v>
       </c>
@@ -20374,8 +20422,11 @@
       <c r="G71" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H71" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>70</v>
       </c>
@@ -20397,8 +20448,11 @@
       <c r="G72" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H72" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <v>71</v>
       </c>
@@ -20420,8 +20474,11 @@
       <c r="G73" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H73" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>72</v>
       </c>
@@ -20443,8 +20500,11 @@
       <c r="G74" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H74" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <v>73</v>
       </c>
@@ -20466,8 +20526,11 @@
       <c r="G75" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H75" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>74</v>
       </c>
@@ -20489,8 +20552,11 @@
       <c r="G76" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H76" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <v>75</v>
       </c>
@@ -20512,8 +20578,11 @@
       <c r="G77" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H77" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>76</v>
       </c>
@@ -20535,8 +20604,11 @@
       <c r="G78" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H78" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
         <v>77</v>
       </c>
@@ -20558,8 +20630,11 @@
       <c r="G79" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H79" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <v>78</v>
       </c>
@@ -20581,8 +20656,11 @@
       <c r="G80" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H80" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
         <v>79</v>
       </c>
@@ -20604,8 +20682,11 @@
       <c r="G81" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H81" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <v>80</v>
       </c>
@@ -20628,7 +20709,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
         <v>81</v>
       </c>
@@ -20651,7 +20732,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
         <v>82</v>
       </c>
@@ -20673,8 +20754,11 @@
       <c r="G84" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H84" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
         <v>83</v>
       </c>
@@ -20697,7 +20781,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <v>84</v>
       </c>
@@ -20719,8 +20803,11 @@
       <c r="G86" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H86" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
         <v>85</v>
       </c>
@@ -20743,7 +20830,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
         <v>86</v>
       </c>
@@ -20765,8 +20852,11 @@
       <c r="G88" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H88" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" s="2">
         <v>87</v>
       </c>
@@ -20788,8 +20878,11 @@
       <c r="G89" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H89" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
         <v>88</v>
       </c>
@@ -20811,8 +20904,11 @@
       <c r="G90" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H90" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="2">
         <v>89</v>
       </c>
@@ -20835,7 +20931,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="2">
         <v>90</v>
       </c>
@@ -20858,7 +20954,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" s="2">
         <v>91</v>
       </c>
@@ -20880,8 +20976,11 @@
       <c r="G93" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H93" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" s="2">
         <v>92</v>
       </c>
@@ -20903,8 +21002,11 @@
       <c r="G94" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H94" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" s="2">
         <v>93</v>
       </c>
@@ -20926,8 +21028,11 @@
       <c r="G95" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H95" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
         <v>94</v>
       </c>
@@ -20949,8 +21054,11 @@
       <c r="G96" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H96" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" s="2">
         <v>95</v>
       </c>
@@ -20972,8 +21080,11 @@
       <c r="G97" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H97" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" s="2">
         <v>96</v>
       </c>
@@ -20995,8 +21106,11 @@
       <c r="G98" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H98" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" s="2">
         <v>97</v>
       </c>
@@ -21018,8 +21132,11 @@
       <c r="G99" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H99" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" s="2">
         <v>98</v>
       </c>
@@ -21041,8 +21158,11 @@
       <c r="G100" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H100" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" s="2">
         <v>99</v>
       </c>
@@ -21064,8 +21184,11 @@
       <c r="G101" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H101" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" s="2">
         <v>100</v>
       </c>
@@ -21087,8 +21210,11 @@
       <c r="G102" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H102" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" s="2">
         <v>101</v>
       </c>
@@ -21110,8 +21236,11 @@
       <c r="G103" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H103" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" s="2">
         <v>102</v>
       </c>
@@ -21133,8 +21262,11 @@
       <c r="G104" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H104" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" s="2">
         <v>103</v>
       </c>
@@ -21156,8 +21288,11 @@
       <c r="G105" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H105" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" s="2">
         <v>104</v>
       </c>
@@ -21179,8 +21314,11 @@
       <c r="G106" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H106" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" s="2">
         <v>105</v>
       </c>
@@ -21202,8 +21340,11 @@
       <c r="G107" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H107" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" s="2">
         <v>106</v>
       </c>
@@ -21225,8 +21366,11 @@
       <c r="G108" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H108" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" s="2">
         <v>107</v>
       </c>
@@ -21248,8 +21392,11 @@
       <c r="G109" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H109" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" s="2">
         <v>108</v>
       </c>
@@ -21271,8 +21418,11 @@
       <c r="G110" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H110" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" s="2">
         <v>109</v>
       </c>
@@ -21294,8 +21444,11 @@
       <c r="G111" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H111" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" s="2">
         <v>110</v>
       </c>
@@ -21317,8 +21470,11 @@
       <c r="G112" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H112" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" s="2">
         <v>111</v>
       </c>
@@ -21340,8 +21496,11 @@
       <c r="G113" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H113" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" s="2">
         <v>112</v>
       </c>
@@ -21363,8 +21522,11 @@
       <c r="G114" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H114" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" s="2">
         <v>113</v>
       </c>
@@ -21386,8 +21548,11 @@
       <c r="G115" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H115" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116" s="2">
         <v>114</v>
       </c>
@@ -21409,8 +21574,11 @@
       <c r="G116" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H116" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117" s="2">
         <v>115</v>
       </c>
@@ -21432,8 +21600,11 @@
       <c r="G117" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H117" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118" s="2">
         <v>116</v>
       </c>
@@ -21455,10 +21626,14 @@
       <c r="G118" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="H118" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="B1:G118" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="A1:H1 A510:H1048576 F17:G24 F15:G15 B25:G509 C14:E16 B14 B2:E13 H15:H509 F2:H14 A2:A509">
+  <conditionalFormatting sqref="A1:H1 A510:H1048576 F17:G24 B25:G509 C14:E16 B14 B2:E13 F2:G15 A2:A509 H2:H509">
     <cfRule type="expression" dxfId="12" priority="9">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>

</xml_diff>

<commit_message>
updated algorithm to include single keyword names
</commit_message>
<xml_diff>
--- a/name_generator/dict/algorithms/algorithm_list.xlsx
+++ b/name_generator/dict/algorithms/algorithm_list.xlsx
@@ -1,27 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/masayukikishi/Dropbox/masayuki_kishi/repositories/create_names_v2/name_generator/dict/algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1732CB7-CF0E-D344-9EF7-89ECE711C35B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABD6A61-5B21-AF4D-AA8E-C1CFF038EFBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20780" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="algorithms" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="7" r:id="rId2"/>
     <sheet name="options" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="8" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">algorithms!$B$1:$B$133</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">algorithms!$A$1:$H$157</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet2!$B$1:$B$47</definedName>
     <definedName name="algorithms_combined_2x2">[1]algorithms_combined!$B$2:$AA$22</definedName>
     <definedName name="algorithms_combined_3x3">[1]algorithms_combined!$AE$2:$CJ$91</definedName>
     <definedName name="three_word_algo">[1]algorithm_types_POS!$C$11:$G$33</definedName>
@@ -47,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="29">
   <si>
     <t>deactivate</t>
   </si>
@@ -131,6 +133,9 @@
   </si>
   <si>
     <t>ffun</t>
+  </si>
+  <si>
+    <t>ms_cut</t>
   </si>
 </sst>
 </file>
@@ -222,7 +227,24 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD9D9D9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -18660,10 +18682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AML133"/>
+  <dimension ref="A1:AML157"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G167" sqref="G167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -18783,13 +18805,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -18799,102 +18815,59 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>18</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>18</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>20</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>18</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>25</v>
@@ -18903,13 +18876,12 @@
         <v>1</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -18917,7 +18889,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>8</v>
@@ -18926,21 +18898,17 @@
         <v>1</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>18</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>25</v>
@@ -18949,13 +18917,12 @@
         <v>1</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -18963,23 +18930,19 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>18</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
@@ -18989,19 +18952,18 @@
         <v>6</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -19009,7 +18971,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>8</v>
@@ -19018,21 +18980,17 @@
         <v>1</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>18</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>8</v>
@@ -19041,37 +18999,29 @@
         <v>1</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>18</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="E19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>18</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
@@ -19081,19 +19031,18 @@
         <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -19101,118 +19050,95 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>20</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="E22" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="E23" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="E24" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="E25" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
@@ -19225,17 +19151,13 @@
         <v>8</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
@@ -19248,133 +19170,110 @@
         <v>8</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>26</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="E28" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>27</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>28</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>29</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>20</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>30</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="G32" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -19383,21 +19282,21 @@
         <v>31</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F33" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="G33" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -19406,22 +19305,25 @@
         <v>32</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F34" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="G34" s="1" t="s">
         <v>18</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
@@ -19429,21 +19331,21 @@
         <v>33</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F35" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="G35" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -19452,21 +19354,21 @@
         <v>34</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F36" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="G36" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -19475,21 +19377,21 @@
         <v>35</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="F37" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="G37" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -19498,21 +19400,21 @@
         <v>36</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F38" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="G38" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -19521,21 +19423,21 @@
         <v>37</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E39" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="F39" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G39" s="2" t="s">
+      <c r="G39" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -19544,25 +19446,22 @@
         <v>38</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="F40" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G40" s="2" t="s">
+      <c r="G40" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
@@ -19570,21 +19469,21 @@
         <v>39</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="F41" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G41" s="2" t="s">
+      <c r="G41" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -19593,21 +19492,21 @@
         <v>40</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="F42" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="G42" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -19616,21 +19515,21 @@
         <v>41</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="F43" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G43" s="2" t="s">
+      <c r="G43" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -19639,21 +19538,21 @@
         <v>42</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="F44" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G44" s="2" t="s">
+      <c r="G44" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -19662,13 +19561,13 @@
         <v>43</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>8</v>
@@ -19678,6 +19577,9 @@
       </c>
       <c r="G45" s="2" t="s">
         <v>18</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
@@ -19685,13 +19587,13 @@
         <v>44</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>8</v>
@@ -19708,13 +19610,13 @@
         <v>45</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>8</v>
@@ -19724,9 +19626,6 @@
       </c>
       <c r="G47" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="H47" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
@@ -19734,13 +19633,13 @@
         <v>46</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>8</v>
@@ -19757,13 +19656,13 @@
         <v>47</v>
       </c>
       <c r="B49" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>8</v>
@@ -19773,9 +19672,6 @@
       </c>
       <c r="G49" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
@@ -19783,13 +19679,13 @@
         <v>48</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>8</v>
@@ -19799,9 +19695,6 @@
       </c>
       <c r="G50" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
@@ -19809,13 +19702,13 @@
         <v>49</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>8</v>
@@ -19832,25 +19725,22 @@
         <v>50</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="H52" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
@@ -19858,13 +19748,13 @@
         <v>51</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>8</v>
@@ -19881,13 +19771,13 @@
         <v>52</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>8</v>
@@ -19897,9 +19787,6 @@
       </c>
       <c r="G54" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="H54" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
@@ -19907,16 +19794,25 @@
         <v>53</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
@@ -19924,19 +19820,22 @@
         <v>54</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H56" s="2" t="s">
-        <v>20</v>
+      <c r="F56" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
@@ -19944,16 +19843,22 @@
         <v>55</v>
       </c>
       <c r="B57" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D57" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C57" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="E57" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
@@ -19961,19 +19866,22 @@
         <v>56</v>
       </c>
       <c r="B58" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C58" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="E58" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H58" s="2" t="s">
-        <v>20</v>
+      <c r="F58" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
@@ -19981,16 +19889,22 @@
         <v>57</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
@@ -19998,16 +19912,22 @@
         <v>58</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
@@ -20015,16 +19935,22 @@
         <v>59</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
@@ -20032,16 +19958,22 @@
         <v>60</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
@@ -20049,19 +19981,22 @@
         <v>61</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H63" s="2" t="s">
-        <v>20</v>
+      <c r="F63" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
@@ -20069,16 +20004,25 @@
         <v>62</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
@@ -20086,13 +20030,13 @@
         <v>63</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>8</v>
@@ -20109,25 +20053,22 @@
         <v>64</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H66" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
@@ -20135,25 +20076,22 @@
         <v>65</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H67" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
@@ -20161,25 +20099,22 @@
         <v>66</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H68" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
@@ -20187,25 +20122,22 @@
         <v>67</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H69" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
@@ -20213,25 +20145,22 @@
         <v>68</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H70" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
@@ -20239,22 +20168,22 @@
         <v>69</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="H71" s="2" t="s">
         <v>20</v>
@@ -20268,22 +20197,19 @@
         <v>1</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H72" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
@@ -20291,22 +20217,22 @@
         <v>71</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="H73" s="2" t="s">
         <v>20</v>
@@ -20317,22 +20243,22 @@
         <v>72</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="H74" s="2" t="s">
         <v>20</v>
@@ -20343,25 +20269,22 @@
         <v>73</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H75" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.3">
@@ -20369,22 +20292,22 @@
         <v>74</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="H76" s="2" t="s">
         <v>20</v>
@@ -20395,25 +20318,22 @@
         <v>75</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H77" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
@@ -20421,22 +20341,22 @@
         <v>76</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="H78" s="2" t="s">
         <v>20</v>
@@ -20453,15 +20373,9 @@
         <v>8</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F79" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G79" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -20476,15 +20390,9 @@
         <v>8</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F80" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G80" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H80" s="2" t="s">
@@ -20499,22 +20407,13 @@
         <v>2</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="F81" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G81" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H81" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.3">
@@ -20522,22 +20421,19 @@
         <v>80</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F82" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G82" s="2" t="s">
-        <v>8</v>
+      <c r="H82" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.3">
@@ -20545,25 +20441,16 @@
         <v>81</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="F83" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G83" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H83" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
@@ -20571,21 +20458,15 @@
         <v>82</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F84" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G84" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -20594,25 +20475,16 @@
         <v>83</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F85" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G85" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H85" s="2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.3">
@@ -20620,25 +20492,16 @@
         <v>84</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G86" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H86" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.3">
@@ -20646,21 +20509,15 @@
         <v>85</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F87" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G87" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H87" s="2" t="s">
@@ -20672,25 +20529,16 @@
         <v>86</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="F88" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G88" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H88" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.3">
@@ -20698,25 +20546,22 @@
         <v>87</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H89" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.3">
@@ -20730,16 +20575,16 @@
         <v>25</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="H90" s="2" t="s">
         <v>20</v>
@@ -20753,16 +20598,16 @@
         <v>1</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="G91" s="2" t="s">
         <v>8</v>
@@ -20776,19 +20621,19 @@
         <v>90</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="G92" s="2" t="s">
         <v>8</v>
@@ -20802,19 +20647,19 @@
         <v>91</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="G93" s="2" t="s">
         <v>8</v>
@@ -20828,19 +20673,19 @@
         <v>92</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="G94" s="2" t="s">
         <v>8</v>
@@ -20860,13 +20705,13 @@
         <v>8</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="G95" s="2" t="s">
         <v>8</v>
@@ -20886,13 +20731,13 @@
         <v>25</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="G96" s="2" t="s">
         <v>8</v>
@@ -20912,16 +20757,19 @@
         <v>8</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="G97" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="H97" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
@@ -20935,13 +20783,13 @@
         <v>8</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="G98" s="2" t="s">
         <v>8</v>
@@ -20955,19 +20803,19 @@
         <v>97</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="G99" s="2" t="s">
         <v>8</v>
@@ -20981,22 +20829,25 @@
         <v>98</v>
       </c>
       <c r="B100" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D100" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C100" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D100" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="E100" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="G100" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="H100" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.3">
@@ -21004,19 +20855,19 @@
         <v>99</v>
       </c>
       <c r="B101" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D101" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C101" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D101" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="E101" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="G101" s="2" t="s">
         <v>8</v>
@@ -21030,10 +20881,10 @@
         <v>100</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>13</v>
@@ -21042,10 +20893,13 @@
         <v>8</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="G102" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="H102" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.3">
@@ -21053,25 +20907,22 @@
         <v>101</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D103" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F103" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E103" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F103" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="G103" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="H103" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.3">
@@ -21079,19 +20930,19 @@
         <v>102</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C104" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G104" s="2" t="s">
         <v>8</v>
@@ -21105,7 +20956,7 @@
         <v>103</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C105" s="2" t="s">
         <v>25</v>
@@ -21117,7 +20968,7 @@
         <v>8</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G105" s="2" t="s">
         <v>8</v>
@@ -21131,7 +20982,7 @@
         <v>104</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C106" s="2" t="s">
         <v>8</v>
@@ -21143,7 +20994,7 @@
         <v>8</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G106" s="2" t="s">
         <v>8</v>
@@ -21154,10 +21005,10 @@
         <v>105</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>13</v>
@@ -21166,7 +21017,7 @@
         <v>8</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G107" s="2" t="s">
         <v>8</v>
@@ -21180,25 +21031,22 @@
         <v>106</v>
       </c>
       <c r="B108" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F108" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C108" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D108" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E108" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F108" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="G108" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="H108" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.3">
@@ -21215,10 +21063,10 @@
         <v>1</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="G109" s="2" t="s">
         <v>8</v>
@@ -21235,7 +21083,7 @@
         <v>1</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>1</v>
@@ -21244,7 +21092,7 @@
         <v>8</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="G110" s="2" t="s">
         <v>8</v>
@@ -21258,7 +21106,7 @@
         <v>109</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="C111" s="2" t="s">
         <v>8</v>
@@ -21270,7 +21118,7 @@
         <v>8</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="G111" s="2" t="s">
         <v>8</v>
@@ -21284,19 +21132,19 @@
         <v>110</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D112" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="G112" s="2" t="s">
         <v>8</v>
@@ -21310,10 +21158,10 @@
         <v>111</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D113" s="2" t="s">
         <v>1</v>
@@ -21322,7 +21170,7 @@
         <v>8</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="G113" s="2" t="s">
         <v>8</v>
@@ -21336,19 +21184,19 @@
         <v>112</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="G114" s="2" t="s">
         <v>8</v>
@@ -21362,19 +21210,19 @@
         <v>113</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="G115" s="2" t="s">
         <v>8</v>
@@ -21388,19 +21236,19 @@
         <v>114</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="G116" s="2" t="s">
         <v>8</v>
@@ -21414,19 +21262,19 @@
         <v>115</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C117" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="G117" s="2" t="s">
         <v>8</v>
@@ -21446,13 +21294,13 @@
         <v>8</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="G118" s="2" t="s">
         <v>8</v>
@@ -21466,19 +21314,19 @@
         <v>117</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D119" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F119" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="E119" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F119" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="G119" s="2" t="s">
         <v>8</v>
@@ -21495,16 +21343,16 @@
         <v>1</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D120" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F120" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="E120" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F120" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="G120" s="2" t="s">
         <v>8</v>
@@ -21518,25 +21366,22 @@
         <v>119</v>
       </c>
       <c r="B121" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F121" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C121" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D121" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E121" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F121" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="G121" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="H121" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.3">
@@ -21544,19 +21389,19 @@
         <v>120</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D122" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F122" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="E122" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F122" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="G122" s="2" t="s">
         <v>8</v>
@@ -21573,16 +21418,16 @@
         <v>2</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D123" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F123" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="E123" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F123" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="G123" s="2" t="s">
         <v>8</v>
@@ -21596,25 +21441,22 @@
         <v>122</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D124" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F124" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E124" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F124" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="G124" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="H124" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.3">
@@ -21625,16 +21467,16 @@
         <v>6</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D125" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F125" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="E125" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F125" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="G125" s="2" t="s">
         <v>8</v>
@@ -21648,25 +21490,22 @@
         <v>124</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C126" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D126" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E126" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F126" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E126" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F126" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="G126" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="H126" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.3">
@@ -21674,19 +21513,19 @@
         <v>125</v>
       </c>
       <c r="B127" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D127" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C127" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D127" s="2" t="s">
+      <c r="E127" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F127" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="E127" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F127" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="G127" s="2" t="s">
         <v>8</v>
@@ -21700,19 +21539,19 @@
         <v>126</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D128" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E128" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F128" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="E128" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F128" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="G128" s="2" t="s">
         <v>8</v>
@@ -21729,16 +21568,16 @@
         <v>1</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D129" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E129" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F129" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="E129" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F129" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="G129" s="2" t="s">
         <v>8</v>
@@ -21752,25 +21591,22 @@
         <v>128</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="C130" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D130" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E130" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F130" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E130" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F130" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="G130" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="H130" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.3">
@@ -21778,19 +21614,19 @@
         <v>129</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C131" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D131" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F131" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="E131" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F131" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="G131" s="2" t="s">
         <v>8</v>
@@ -21804,16 +21640,16 @@
         <v>130</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="F132" s="2" t="s">
         <v>11</v>
@@ -21830,13 +21666,13 @@
         <v>131</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>8</v>
@@ -21851,32 +21687,660 @@
         <v>20</v>
       </c>
     </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A134" s="2">
+        <v>132</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E134" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F134" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G134" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H134" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A135" s="2">
+        <v>133</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D135" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E135" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F135" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G135" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H135" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A136" s="2">
+        <v>134</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D136" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E136" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F136" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G136" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H136" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A137" s="2">
+        <v>135</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D137" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E137" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F137" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G137" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H137" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A138" s="2">
+        <v>136</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D138" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E138" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F138" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G138" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H138" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A139" s="2">
+        <v>137</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D139" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E139" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F139" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G139" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H139" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A140" s="2">
+        <v>138</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D140" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E140" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F140" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G140" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H140" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A141" s="2">
+        <v>139</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D141" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E141" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F141" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G141" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H141" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A142" s="2">
+        <v>140</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D142" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E142" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F142" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G142" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H142" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A143" s="2">
+        <v>141</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D143" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E143" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F143" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G143" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H143" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A144" s="2">
+        <v>142</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D144" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E144" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F144" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G144" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H144" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A145" s="2">
+        <v>143</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D145" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E145" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F145" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G145" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H145" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A146" s="2">
+        <v>144</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E146" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F146" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G146" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H146" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A147" s="2">
+        <v>145</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D147" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E147" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F147" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G147" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H147" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A148" s="2">
+        <v>146</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D148" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E148" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F148" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G148" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H148" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A149" s="2">
+        <v>147</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E149" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F149" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G149" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H149" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A150" s="2">
+        <v>148</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E150" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F150" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G150" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H150" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A151" s="2">
+        <v>149</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D151" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E151" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F151" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G151" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H151" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A152" s="2">
+        <v>150</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D152" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E152" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F152" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G152" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H152" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A153" s="2">
+        <v>151</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D153" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E153" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F153" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G153" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H153" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A154" s="2">
+        <v>152</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D154" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E154" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F154" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G154" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H154" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A155" s="2">
+        <v>153</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D155" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E155" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F155" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G155" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H155" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A156" s="2">
+        <v>154</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D156" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E156" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F156" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G156" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H156" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A157" s="2">
+        <v>155</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D157" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E157" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F157" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G157" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H157" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="B1:B133" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="A1:H1 F22:G29 C19:E21 B19 B30:G60 F61:G61 C62:G64 B61:B64 A134:H1048576 F2:G20 H2:H64 A2:E3 B4:E18 B65:H133 A4:A133">
-    <cfRule type="expression" dxfId="0" priority="10">
+  <conditionalFormatting sqref="A1:H1 A2:E3 B89:H157 A158:H1048576 H2:H88 F2:G45 A4:A157">
+    <cfRule type="expression" dxfId="10" priority="13">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B22:E29 B20:B21">
-    <cfRule type="expression" dxfId="7" priority="6">
-      <formula>LEN(TRIM(B20))=0</formula>
+  <conditionalFormatting sqref="B4:E6 B31:E45 D7:E11 B9:B11">
+    <cfRule type="expression" dxfId="9" priority="9">
+      <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F21">
-    <cfRule type="expression" dxfId="6" priority="3">
-      <formula>LEN(TRIM(F21))=0</formula>
+  <conditionalFormatting sqref="B46:G88">
+    <cfRule type="expression" dxfId="8" priority="4">
+      <formula>LEN(TRIM(B46))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G21">
-    <cfRule type="expression" dxfId="5" priority="2">
-      <formula>LEN(TRIM(G21))=0</formula>
+  <conditionalFormatting sqref="B7:C7 B8 C8:C11">
+    <cfRule type="expression" dxfId="7" priority="3">
+      <formula>LEN(TRIM(B7))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C61:E61">
-    <cfRule type="expression" dxfId="4" priority="1">
-      <formula>LEN(TRIM(C61))=0</formula>
+  <conditionalFormatting sqref="B12:D20 E12:E30">
+    <cfRule type="expression" dxfId="6" priority="2">
+      <formula>LEN(TRIM(B12))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21:D30">
+    <cfRule type="expression" dxfId="5" priority="1">
+      <formula>LEN(TRIM(B21))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -22095,22 +22559,388 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:B6 A2:D4 C1:D1 E1:F2">
+  <conditionalFormatting sqref="C5:D7">
+    <cfRule type="expression" dxfId="4" priority="1">
+      <formula>LEN(TRIM(C5))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:F2 A1:D4 A5:B6">
     <cfRule type="expression" dxfId="3" priority="2">
       <formula>LEN(TRIM(A1))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:B1">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>LEN(TRIM(A1))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C5:D7">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>LEN(TRIM(C5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{231D618F-E04E-4E44-A52E-C579D0F18948}">
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="str">
+        <f>_xlfn.CONCAT(A1,",",B1,",",C1,",",D1)</f>
+        <v>noun,ab_cut,noun,ms_cut</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" t="str">
+        <f t="shared" ref="E2:E19" si="0">_xlfn.CONCAT(A2,",",B2,",",C2,",",D2)</f>
+        <v>noun,no_cut,noun,ms_cut</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" si="0"/>
+        <v>verb,ab_cut,noun,ms_cut</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>verb,no_cut,noun,ms_cut</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>adje,ab_cut,noun,ms_cut</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>adje,no_cut,noun,ms_cut</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>pref,no_cut,noun,ms_cut</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v>head,no_cut,noun,ms_cut</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="0"/>
+        <v>noun,ab_cut,verb,ms_cut</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="0"/>
+        <v>noun,no_cut,verb,ms_cut</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="0"/>
+        <v>pref,no_cut,verb,ms_cut</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="0"/>
+        <v>head,no_cut,verb,ms_cut</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="0"/>
+        <v>pref,no_cut,adje,ms_cut</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="0"/>
+        <v>head,no_cut,adje,ms_cut</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="0"/>
+        <v>pref,no_cut,advb,ms_cut</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="0"/>
+        <v>head,no_cut,advb,ms_cut</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="0"/>
+        <v>ffun,no_cut,noun,ms_cut</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="0"/>
+        <v>ffun,no_cut,verb,ms_cut</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="0"/>
+        <v>ffun,no_cut,advb,ms_cut</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:B47" xr:uid="{231D618F-E04E-4E44-A52E-C579D0F18948}"/>
+  <conditionalFormatting sqref="A1:C9 D1:D19">
+    <cfRule type="expression" dxfId="2" priority="5">
+      <formula>LEN(TRIM(A1))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10:C19">
+    <cfRule type="expression" dxfId="1" priority="4">
+      <formula>LEN(TRIM(A10))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated googltrans and requirements
</commit_message>
<xml_diff>
--- a/name_generator/dict/algorithms/algorithm_list.xlsx
+++ b/name_generator/dict/algorithms/algorithm_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/masayukikishi/Dropbox/masayuki_kishi/repositories/create_names_v2/name_generator/dict/algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABD6A61-5B21-AF4D-AA8E-C1CFF038EFBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474FBB87-396F-B540-B991-F31E614DE39C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20780" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="algorithms" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1089" uniqueCount="29">
   <si>
     <t>deactivate</t>
   </si>
@@ -227,7 +227,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="7">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -235,34 +235,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9D9D9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9D9D9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9D9D9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9D9D9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -18684,8 +18656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AML157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G167" sqref="G167"/>
+    <sheetView tabSelected="1" topLeftCell="A133" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J151" sqref="J151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -18902,6 +18874,9 @@
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
+      <c r="H13" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
@@ -18943,6 +18918,9 @@
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
+      <c r="H15" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
@@ -18984,6 +18962,9 @@
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
+      <c r="H17" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
@@ -19003,6 +18984,9 @@
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
+      <c r="H18" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
@@ -19022,6 +19006,9 @@
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
+      <c r="H19" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
@@ -19063,6 +19050,9 @@
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
+      <c r="H21" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
@@ -19082,6 +19072,9 @@
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
+      <c r="H22" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
@@ -19101,6 +19094,9 @@
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
+      <c r="H23" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
@@ -19120,6 +19116,9 @@
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
+      <c r="H24" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
@@ -19139,6 +19138,9 @@
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
+      <c r="H25" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
@@ -19158,6 +19160,9 @@
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
+      <c r="H26" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
@@ -19177,6 +19182,9 @@
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
+      <c r="H27" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
@@ -19196,6 +19204,9 @@
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
+      <c r="H28" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
@@ -19215,6 +19226,9 @@
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
+      <c r="H29" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
@@ -19234,6 +19248,9 @@
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
+      <c r="H30" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
@@ -19253,6 +19270,9 @@
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
+      <c r="H31" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
@@ -19276,6 +19296,9 @@
       <c r="G32" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="H32" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
@@ -19299,6 +19322,9 @@
       <c r="G33" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="H33" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
@@ -19348,6 +19374,9 @@
       <c r="G35" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="H35" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
@@ -19371,6 +19400,9 @@
       <c r="G36" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="H36" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
@@ -19394,6 +19426,9 @@
       <c r="G37" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="H37" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
@@ -19417,6 +19452,9 @@
       <c r="G38" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="H38" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
@@ -19440,6 +19478,9 @@
       <c r="G39" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="H39" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
@@ -19463,6 +19504,9 @@
       <c r="G40" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="H40" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
@@ -19486,6 +19530,9 @@
       <c r="G41" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="H41" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
@@ -19509,6 +19556,9 @@
       <c r="G42" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="H42" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
@@ -19532,6 +19582,9 @@
       <c r="G43" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="H43" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
@@ -19555,6 +19608,9 @@
       <c r="G44" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="H44" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
@@ -19604,6 +19660,9 @@
       <c r="G46" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="H46" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
@@ -19627,6 +19686,9 @@
       <c r="G47" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="H47" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
@@ -19650,6 +19712,9 @@
       <c r="G48" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="H48" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
@@ -19673,6 +19738,9 @@
       <c r="G49" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="H49" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
@@ -19696,6 +19764,9 @@
       <c r="G50" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="H50" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
@@ -19719,6 +19790,9 @@
       <c r="G51" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="H51" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
@@ -19742,6 +19816,9 @@
       <c r="G52" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="H52" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
@@ -19765,6 +19842,9 @@
       <c r="G53" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="H53" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
@@ -19788,6 +19868,9 @@
       <c r="G54" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="H54" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
@@ -19837,6 +19920,9 @@
       <c r="G56" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="H56" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
@@ -19860,6 +19946,9 @@
       <c r="G57" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="H57" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
@@ -19883,6 +19972,9 @@
       <c r="G58" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="H58" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
@@ -19906,6 +19998,9 @@
       <c r="G59" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="H59" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
@@ -19929,6 +20024,9 @@
       <c r="G60" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="H60" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
@@ -19952,6 +20050,9 @@
       <c r="G61" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="H61" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
@@ -19975,6 +20076,9 @@
       <c r="G62" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="H62" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
@@ -19998,6 +20102,9 @@
       <c r="G63" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="H63" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
@@ -20047,6 +20154,9 @@
       <c r="G65" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="H65" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
@@ -20070,6 +20180,9 @@
       <c r="G66" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="H66" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
@@ -20093,6 +20206,9 @@
       <c r="G67" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="H67" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
@@ -20116,6 +20232,9 @@
       <c r="G68" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="H68" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
@@ -20139,6 +20258,9 @@
       <c r="G69" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="H69" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
@@ -20162,6 +20284,9 @@
       <c r="G70" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="H70" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
@@ -20211,6 +20336,9 @@
       <c r="G72" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="H72" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
@@ -20286,6 +20414,9 @@
       <c r="G75" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="H75" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
@@ -20335,6 +20466,9 @@
       <c r="G77" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="H77" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
@@ -20378,6 +20512,9 @@
       <c r="E79" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="H79" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
@@ -20415,6 +20552,9 @@
       <c r="E81" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="H81" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
@@ -20452,6 +20592,9 @@
       <c r="E83" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="H83" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
@@ -20469,6 +20612,9 @@
       <c r="E84" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="H84" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
@@ -20486,6 +20632,9 @@
       <c r="E85" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="H85" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
@@ -20503,6 +20652,9 @@
       <c r="E86" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="H86" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
@@ -20540,6 +20692,9 @@
       <c r="E88" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="H88" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" s="2">
@@ -20563,6 +20718,9 @@
       <c r="G89" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="H89" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
@@ -20924,6 +21082,9 @@
       <c r="G103" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="H103" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" s="2">
@@ -20999,6 +21160,9 @@
       <c r="G106" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="H106" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" s="2">
@@ -21048,6 +21212,9 @@
       <c r="G108" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="H108" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" s="2">
@@ -21383,6 +21550,9 @@
       <c r="G121" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="H121" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" s="2">
@@ -21458,6 +21628,9 @@
       <c r="G124" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="H124" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" s="2">
@@ -21507,6 +21680,9 @@
       <c r="G126" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="H126" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127" s="2">
@@ -21608,6 +21784,9 @@
       <c r="G130" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="H130" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131" s="2">
@@ -22313,34 +22492,19 @@
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="A1:H1 A2:E3 B89:H157 A158:H1048576 H2:H88 F2:G45 A4:A157">
-    <cfRule type="expression" dxfId="10" priority="13">
+  <conditionalFormatting sqref="A1:H1 A2:E3 F2:G45 A4:A157 B89:G157 A158:H1048576 H2:H157">
+    <cfRule type="expression" dxfId="6" priority="13">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4:E6 B31:E45 D7:E11 B9:B11">
-    <cfRule type="expression" dxfId="9" priority="9">
+  <conditionalFormatting sqref="B4:E45">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46:G88">
-    <cfRule type="expression" dxfId="8" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>LEN(TRIM(B46))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7:C7 B8 C8:C11">
-    <cfRule type="expression" dxfId="7" priority="3">
-      <formula>LEN(TRIM(B7))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B12:D20 E12:E30">
-    <cfRule type="expression" dxfId="6" priority="2">
-      <formula>LEN(TRIM(B12))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B21:D30">
-    <cfRule type="expression" dxfId="5" priority="1">
-      <formula>LEN(TRIM(B21))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -22560,12 +22724,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:D7">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>LEN(TRIM(C5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:F2 A1:D4 A5:B6">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22928,14 +23092,9 @@
     </row>
   </sheetData>
   <autoFilter ref="B1:B47" xr:uid="{231D618F-E04E-4E44-A52E-C579D0F18948}"/>
-  <conditionalFormatting sqref="A1:C9 D1:D19">
-    <cfRule type="expression" dxfId="2" priority="5">
+  <conditionalFormatting sqref="A1:D19">
+    <cfRule type="expression" dxfId="1" priority="4">
       <formula>LEN(TRIM(A1))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A10:C19">
-    <cfRule type="expression" dxfId="1" priority="4">
-      <formula>LEN(TRIM(A10))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">

</xml_diff>